<commit_message>
changed RH service period to 10 years from 70
</commit_message>
<xml_diff>
--- a/ruleconfig/Rule Specification.xlsx
+++ b/ruleconfig/Rule Specification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420"/>
   </bookViews>
   <sheets>
     <sheet name="RH" sheetId="1" r:id="rId1"/>
@@ -1109,9 +1109,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F137" sqref="F137"/>
+      <selection pane="bottomLeft" activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,7 +1958,7 @@
         <v>28</v>
       </c>
       <c r="J38" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O38" s="7"/>
       <c r="P38" s="7"/>
@@ -1992,7 +1992,7 @@
         <v>21</v>
       </c>
       <c r="J39" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O39" s="7"/>
     </row>
@@ -2025,7 +2025,7 @@
         <v>7</v>
       </c>
       <c r="J40" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O40" s="7"/>
     </row>
@@ -2059,7 +2059,7 @@
         <v>161</v>
       </c>
       <c r="J41" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O41" s="7"/>
     </row>
@@ -2093,7 +2093,7 @@
         <v>182</v>
       </c>
       <c r="J42" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O42" s="7"/>
     </row>
@@ -2127,7 +2127,7 @@
         <v>28</v>
       </c>
       <c r="J43" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O43" s="7"/>
     </row>
@@ -2412,7 +2412,7 @@
         <v>28</v>
       </c>
       <c r="J56" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O56" s="7"/>
     </row>
@@ -2445,7 +2445,7 @@
         <v>21</v>
       </c>
       <c r="J57" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O57" s="7"/>
     </row>
@@ -2478,7 +2478,7 @@
         <v>7</v>
       </c>
       <c r="J58" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O58" s="7"/>
     </row>
@@ -2505,7 +2505,7 @@
         <v>161</v>
       </c>
       <c r="J59" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O59" s="7"/>
     </row>
@@ -2532,7 +2532,7 @@
         <v>182</v>
       </c>
       <c r="J60" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O60" s="7"/>
     </row>
@@ -2565,7 +2565,7 @@
         <v>91</v>
       </c>
       <c r="J61" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O61" s="7"/>
     </row>
@@ -3744,7 +3744,7 @@
         <v>28</v>
       </c>
       <c r="J116" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O116" s="7"/>
     </row>
@@ -3771,7 +3771,7 @@
         <v>21</v>
       </c>
       <c r="J117" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O117" s="7"/>
     </row>
@@ -3798,7 +3798,7 @@
         <v>7</v>
       </c>
       <c r="J118" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O118" s="7"/>
     </row>
@@ -3825,7 +3825,7 @@
         <v>161</v>
       </c>
       <c r="J119" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O119" s="7"/>
     </row>
@@ -3873,7 +3873,7 @@
         <v>182</v>
       </c>
       <c r="J121" s="3">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="O121" s="7"/>
     </row>
@@ -4040,8 +4040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H121"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>